<commit_message>
Uploading latest revision of Database model
Added a lot of extra tables and solidified formatting
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08D2A662-C3A9-4881-AC8F-FE429BA8FD77}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56CEAEC0-F8BC-4037-8590-5AFDDAFAA4C9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{E1E5376B-4DE1-467A-861F-B4D1BD91DE5C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6420" xr2:uid="{D0CF116F-F494-4758-8B2C-D2FC8A09A9E9}"/>
   </bookViews>
   <sheets>
     <sheet name="TestFile" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Comment</t>
   </si>
@@ -40,30 +40,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Supplier 1</t>
-  </si>
-  <si>
-    <t>Supplier Currency 1</t>
-  </si>
-  <si>
-    <t>Supplier Part Number 1</t>
-  </si>
-  <si>
-    <t>Supplier Stock 1</t>
-  </si>
-  <si>
-    <t>Supplier Unit Price 1</t>
-  </si>
-  <si>
-    <t>Capacitance</t>
-  </si>
-  <si>
-    <t>Resistance</t>
-  </si>
-  <si>
     <t>0402 0.1uF Cap</t>
   </si>
   <si>
@@ -79,45 +55,18 @@
     <t>2001</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL05F104ZO5NNNC/1276-1004-1-ND/3889090</t>
-  </si>
-  <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>1276-1004-1-ND</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>0402 Resistor</t>
   </si>
   <si>
     <t>10 kOhms ±1% 0.2W, 1/5W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200, Pulse Withstanding Thick Film</t>
   </si>
   <si>
-    <t>R1, R2, R4</t>
+    <t>R1, R2, R4, R5, R6, R7, R8, R9, R10</t>
   </si>
   <si>
     <t>1001</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PA2F1002X/P17230TR-ND/5402656</t>
-  </si>
-  <si>
-    <t>P17230TR-ND</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
     <t>1% 0402 Resistor thing</t>
   </si>
   <si>
@@ -128,19 +77,13 @@
   </si>
   <si>
     <t>1002</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/vishay-beyschlag/MCS04020C1002FE000/MCS0402-10.0K-CFCT-ND/2607929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCS0402-10.0K-CFCT-ND	</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,14 +96,6 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -201,21 +136,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,17 +459,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895F1532-9E4C-466C-9A8D-BE4D2361ACBC}">
-  <dimension ref="A1:N4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD14FD0-D351-41CA-9DAB-DC42EEC6DCCF}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="14.42578125" customWidth="1"/>
+    <col min="1" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,166 +488,69 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="3">
-        <v>100000</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" tooltip="Supplier" display="'1276-1004-1-ND" xr:uid="{45CA728A-8F4C-4494-A229-C11024C52ACA}"/>
-    <hyperlink ref="J3" r:id="rId2" tooltip="Supplier" display="'P17230TR-ND" xr:uid="{8B79D4AA-6BBD-43B3-8BC8-3FA4BF909018}"/>
-    <hyperlink ref="J4" tooltip="Supplier" display="'MCS0402-10.0K-CFCT-ND_x0009_" xr:uid="{1B0DBA2A-F23C-46BD-9A59-C4490B8517A0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>